<commit_message>
Fixed minor error in BOM.
</commit_message>
<xml_diff>
--- a/EE/v1.0/RCM-PBB_E1_BOM_9_25_15.xlsx
+++ b/EE/v1.0/RCM-PBB_E1_BOM_9_25_15.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="17030"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Donna\Desktop\RCM-PBB_E1\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1125" yWindow="-15" windowWidth="19545" windowHeight="11760"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23700" windowHeight="8130"/>
   </bookViews>
   <sheets>
     <sheet name="Bus Board BOM" sheetId="1" r:id="rId1"/>
@@ -17,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="174">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="193" uniqueCount="173">
   <si>
     <t>James Yost - jamesyost12@yahoo.com</t>
   </si>
@@ -289,9 +294,6 @@
     <t>RES 1.00M OHM 1/8W 1% 0805 SMD</t>
   </si>
   <si>
-    <t>Bus BD BOM</t>
-  </si>
-  <si>
     <t>J1</t>
   </si>
   <si>
@@ -331,9 +333,6 @@
     <t>1317G18</t>
   </si>
   <si>
-    <t>879-1317G18-BK</t>
-  </si>
-  <si>
     <t>ANDERSON_POWER_POLE RED</t>
   </si>
   <si>
@@ -343,9 +342,6 @@
     <t>ANDERSON_POWER_POLE BLUE WINGS</t>
   </si>
   <si>
-    <t>25A Right Angle Pins</t>
-  </si>
-  <si>
     <t xml:space="preserve">C1,2 </t>
   </si>
   <si>
@@ -355,9 +351,6 @@
     <t>C4,7,8</t>
   </si>
   <si>
-    <t>Basic</t>
-  </si>
-  <si>
     <t>LED3</t>
   </si>
   <si>
@@ -539,13 +532,22 @@
   </si>
   <si>
     <t>MCR10ERTF1000</t>
+  </si>
+  <si>
+    <t>879-1377G4-BK</t>
+  </si>
+  <si>
+    <t>ANDERSON_POWER_25A STRAIGHT PINS</t>
+  </si>
+  <si>
+    <t>RCM-PBB_E1 Bus BD BOM</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="8">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -660,6 +662,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -706,7 +716,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -738,9 +748,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -772,6 +800,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -947,14 +993,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="E43" sqref="E43"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="21.5703125" customWidth="1"/>
     <col min="2" max="3" width="20.7109375" customWidth="1"/>
@@ -965,48 +1011,46 @@
     <col min="13" max="13" width="12.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>112</v>
-      </c>
+        <v>172</v>
+      </c>
+      <c r="B1" s="1"/>
       <c r="C1" s="1"/>
       <c r="D1" s="1"/>
       <c r="E1" s="2">
         <v>42272</v>
       </c>
     </row>
-    <row r="2" spans="1:14">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
     </row>
-    <row r="3" spans="1:14">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="4" spans="1:14">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:14">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:14">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="C6" s="3"/>
     </row>
-    <row r="7" spans="1:14">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" s="3"/>
     </row>
-    <row r="9" spans="1:14">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="G9" s="4"/>
       <c r="N9" s="4"/>
     </row>
-    <row r="10" spans="1:14">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" s="14" t="s">
         <v>2</v>
       </c>
@@ -1034,9 +1078,9 @@
       <c r="K10" s="5"/>
       <c r="L10" s="6"/>
     </row>
-    <row r="11" spans="1:14">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11" s="8" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="B11" s="8" t="s">
         <v>8</v>
@@ -1057,9 +1101,9 @@
         <v>7</v>
       </c>
     </row>
-    <row r="12" spans="1:14">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12" s="9" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="B12" s="8" t="s">
         <v>9</v>
@@ -1080,9 +1124,9 @@
         <v>40</v>
       </c>
     </row>
-    <row r="13" spans="1:14">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A13" s="8" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="B13" s="8" t="s">
         <v>10</v>
@@ -1103,7 +1147,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="14" spans="1:14">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A14" s="8" t="s">
         <v>12</v>
       </c>
@@ -1126,101 +1170,101 @@
         <v>46</v>
       </c>
     </row>
-    <row r="15" spans="1:14">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A15" s="9" t="s">
+        <v>90</v>
+      </c>
+      <c r="B15" s="8" t="s">
         <v>91</v>
       </c>
-      <c r="B15" s="8" t="s">
+      <c r="C15" s="11" t="s">
         <v>92</v>
-      </c>
-      <c r="C15" s="11" t="s">
-        <v>93</v>
       </c>
       <c r="D15" s="12">
         <v>1327</v>
       </c>
       <c r="E15" s="16" t="s">
+        <v>93</v>
+      </c>
+      <c r="F15" s="11">
+        <v>1</v>
+      </c>
+      <c r="G15" s="10" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A16" s="9" t="s">
         <v>94</v>
       </c>
-      <c r="F15" s="11">
-        <v>1</v>
-      </c>
-      <c r="G15" s="10" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="16" spans="1:14">
-      <c r="A16" s="9" t="s">
+      <c r="B16" s="8" t="s">
         <v>95</v>
       </c>
-      <c r="B16" s="8" t="s">
+      <c r="C16" s="11" t="s">
+        <v>92</v>
+      </c>
+      <c r="D16" s="10" t="s">
         <v>96</v>
       </c>
-      <c r="C16" s="11" t="s">
-        <v>93</v>
-      </c>
-      <c r="D16" s="10" t="s">
+      <c r="E16" s="16" t="s">
         <v>97</v>
       </c>
-      <c r="E16" s="16" t="s">
-        <v>98</v>
-      </c>
       <c r="F16" s="11">
         <v>1</v>
       </c>
       <c r="G16" s="10" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="9" t="s">
         <v>13</v>
       </c>
       <c r="B17" s="8" t="s">
+        <v>98</v>
+      </c>
+      <c r="C17" s="11" t="s">
+        <v>92</v>
+      </c>
+      <c r="D17" s="10" t="s">
         <v>99</v>
       </c>
-      <c r="C17" s="11" t="s">
-        <v>93</v>
-      </c>
-      <c r="D17" s="10" t="s">
+      <c r="E17" s="16" t="s">
         <v>100</v>
-      </c>
-      <c r="E17" s="16" t="s">
-        <v>101</v>
       </c>
       <c r="F17" s="11">
         <v>2</v>
       </c>
       <c r="G17" s="10" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="9" t="s">
         <v>13</v>
       </c>
       <c r="B18" s="8" t="s">
+        <v>101</v>
+      </c>
+      <c r="C18" s="11" t="s">
+        <v>92</v>
+      </c>
+      <c r="D18" s="10" t="s">
         <v>102</v>
       </c>
-      <c r="C18" s="11" t="s">
-        <v>93</v>
-      </c>
-      <c r="D18" s="10" t="s">
-        <v>103</v>
-      </c>
       <c r="E18" s="8" t="s">
-        <v>104</v>
+        <v>170</v>
       </c>
       <c r="F18" s="11">
         <v>2</v>
       </c>
       <c r="G18" s="11" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="8" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="B19" s="8" t="s">
         <v>50</v>
@@ -1241,9 +1285,9 @@
         <v>51</v>
       </c>
     </row>
-    <row r="20" spans="1:7">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="8" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="B20" s="8" t="s">
         <v>71</v>
@@ -1264,7 +1308,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="21" spans="1:7">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="8" t="s">
         <v>84</v>
       </c>
@@ -1287,7 +1331,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="22" spans="1:7">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="8" t="s">
         <v>85</v>
       </c>
@@ -1310,7 +1354,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="23" spans="1:7">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="8" t="s">
         <v>15</v>
       </c>
@@ -1333,9 +1377,9 @@
         <v>83</v>
       </c>
     </row>
-    <row r="24" spans="1:7">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="8" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="B24" s="13">
         <v>100</v>
@@ -1344,21 +1388,21 @@
         <v>88</v>
       </c>
       <c r="D24" s="18" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="E24" s="16" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
       <c r="F24" s="11">
         <v>1</v>
       </c>
       <c r="G24" s="8" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="8" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="B25" s="13">
         <v>750</v>
@@ -1367,21 +1411,21 @@
         <v>88</v>
       </c>
       <c r="D25" s="18" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="E25" s="16" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="F25" s="11">
         <v>1</v>
       </c>
       <c r="G25" s="8" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" s="8" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="B26" s="13" t="s">
         <v>16</v>
@@ -1390,21 +1434,21 @@
         <v>88</v>
       </c>
       <c r="D26" s="18" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="E26" s="16" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="F26" s="11">
         <v>3</v>
       </c>
       <c r="G26" s="8" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7" ht="15" customHeight="1">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="8" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="B27" s="13">
         <v>240</v>
@@ -1413,67 +1457,67 @@
         <v>88</v>
       </c>
       <c r="D27" s="18" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="E27" s="16" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="F27" s="11">
         <v>2</v>
       </c>
       <c r="G27" s="8" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7" ht="15" customHeight="1">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="8" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="B28" s="13" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="C28" s="12" t="s">
         <v>88</v>
       </c>
       <c r="D28" s="18" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="E28" s="16" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="F28" s="11">
         <v>1</v>
       </c>
       <c r="G28" s="8" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" s="8" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="B29" s="13" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="C29" s="12" t="s">
         <v>88</v>
       </c>
       <c r="D29" s="18" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="E29" s="16" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="F29" s="11">
         <v>1</v>
       </c>
       <c r="G29" s="8" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="30" spans="1:7">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" s="9" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
       <c r="B30" s="13" t="s">
         <v>17</v>
@@ -1482,42 +1526,42 @@
         <v>88</v>
       </c>
       <c r="D30" s="18" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="E30" s="16" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="F30" s="11">
         <v>2</v>
       </c>
       <c r="G30" s="8" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="31" spans="1:7">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" s="9" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="B31" s="13" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="C31" s="8" t="s">
         <v>88</v>
       </c>
       <c r="D31" s="18" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="E31" s="16" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="F31" s="11">
         <v>1</v>
       </c>
       <c r="G31" s="8" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="32" spans="1:7">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" s="9" t="s">
         <v>19</v>
       </c>
@@ -1528,65 +1572,65 @@
         <v>88</v>
       </c>
       <c r="D32" s="18" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="E32" s="16" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="F32" s="11">
         <v>1</v>
       </c>
       <c r="G32" s="8" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="33" spans="1:7">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" s="9" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="B33" s="13" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="C33" s="8" t="s">
         <v>88</v>
       </c>
       <c r="D33" s="18" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="E33" s="16" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="F33" s="11">
         <v>1</v>
       </c>
       <c r="G33" s="8" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="34" spans="1:7">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" s="9" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="B34" s="13" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="C34" s="8" t="s">
         <v>88</v>
       </c>
       <c r="D34" s="18" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="E34" s="16" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="F34" s="11">
         <v>1</v>
       </c>
       <c r="G34" s="8" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="35" spans="1:7">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" s="9" t="s">
         <v>21</v>
       </c>
@@ -1609,30 +1653,30 @@
         <v>89</v>
       </c>
     </row>
-    <row r="36" spans="1:7">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" s="9" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="B36" s="13" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="C36" s="8" t="s">
         <v>88</v>
       </c>
       <c r="D36" s="18" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="E36" s="16" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="F36" s="11">
         <v>1</v>
       </c>
       <c r="G36" s="8" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="37" spans="1:7">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" s="8" t="s">
         <v>23</v>
       </c>
@@ -1655,7 +1699,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="38" spans="1:7">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38" s="8" t="s">
         <v>25</v>
       </c>
@@ -1678,7 +1722,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="39" spans="1:7">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39" s="8" t="s">
         <v>28</v>
       </c>
@@ -1701,7 +1745,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="40" spans="1:7">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40" s="8" t="s">
         <v>30</v>
       </c>
@@ -1724,30 +1768,30 @@
         <v>58</v>
       </c>
     </row>
-    <row r="41" spans="1:7" ht="15" customHeight="1">
+    <row r="41" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="8" t="s">
         <v>26</v>
       </c>
       <c r="B41" s="8" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="C41" s="8" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="D41" s="11" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="E41" s="16" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="F41" s="11">
         <v>1</v>
       </c>
       <c r="G41" s="8" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="42" spans="1:7" ht="15" customHeight="1">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E42" s="3"/>
     </row>
   </sheetData>
@@ -1800,36 +1844,36 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>